<commit_message>
Finalizando notebook de pré-processamento
</commit_message>
<xml_diff>
--- a/datasets/Chamados_Validação.xlsx
+++ b/datasets/Chamados_Validação.xlsx
@@ -19,28 +19,28 @@
     <t>Descricao Atualizada</t>
   </si>
   <si>
-    <t>dev cumpr estil solicit acess past secret geral estagiár alin cristin dia silv mat numer</t>
-  </si>
-  <si>
-    <t>senh dire cient determin impost cort cont espec cont control relacion seguranç comun v sa exclus serv rafael dia sant cpf numer tod sistem tce rn part dia numer numer numer términ ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informá provid cab</t>
-  </si>
-  <si>
-    <t>senh dire cient determin impost cort cont espec cont control relacion seguranç comun v sa exclus serv mar edelcid gondim doliv cpf numer tod sistem tce rn part dia numer numer numer términ ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informá provid cab</t>
-  </si>
-  <si>
-    <t>cadastr diári ofic tce dat public numer numer numer númer numer ano numer</t>
-  </si>
-  <si>
-    <t>solicit verific possibil cri cham técn recorr útil lembr sobr taref set suport repet form diár mens seman</t>
-  </si>
-  <si>
-    <t>disponibil list complet cham técn ativ soment funcion serv terceir efetiv gerenc cham norm cad serv terceir estagi dev visual soment cham figur solicit atend respons</t>
+    <t>dev cumpr estil solicit acess past secret geral estagiar alin cristin dia silv mat numer</t>
+  </si>
+  <si>
+    <t>senh dire cient determin impost cort cont espec cont control relacion seguranc comun v sa exclus serv rafael dia sant cpf numer tod sistem tce rn part dia numer numer numer termin ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informa provid cab</t>
+  </si>
+  <si>
+    <t>senh dire cient determin impost cort cont espec cont control relacion seguranc comun v sa exclus serv mar edelcid gondim doliv cpf numer tod sistem tce rn part dia numer numer numer termin ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informa provid cab</t>
+  </si>
+  <si>
+    <t>cadastr diari ofic tce dat public numer numer numer numer numer ano numer</t>
+  </si>
+  <si>
+    <t>solicit verific possibil cri cham tecn recorr util lembr sobr taref set suport repet form diar mens seman</t>
+  </si>
+  <si>
+    <t>disponibil list complet cham tecn ativ soment funcion serv terceir efetiv gerenc cham norm cad serv terceir estagi dev visual soment cham figur solicit atend respons</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>solicit cham associ atend pesso apareç list cham ferrament cham gerenci cham pesso mesm form acontec cham pesso vincul solicit destinat</t>
+    <t>solicit cham associ atend pesso aparec list cham ferrament cham gerenci cham pesso mesm form acontec cham pesso vincul solicit destinat</t>
   </si>
   <si>
     <t>comput internet</t>
@@ -61,16 +61,16 @@
     <t>configur wif smartphon serv</t>
   </si>
   <si>
-    <t>estagiár dúv pont biométr</t>
-  </si>
-  <si>
-    <t>solicit presenç técn habil numer doi notebook uso extern tce</t>
+    <t>estagiar duv pont biometr</t>
+  </si>
+  <si>
+    <t>solicit presenc tecn habil numer doi notebook uso extern tce</t>
   </si>
   <si>
     <t>serv aleg mous funcion</t>
   </si>
   <si>
-    <t>verifiq algum despach cadastr mim encontr ativ dispon inclus mal diret emb vis consult lo funcional mal diret cadastr model exempl despach gq desp ice anális</t>
+    <t>verifiq algum despach cadastr mim encontr ativ dispon inclus mal diret emb vis consult lo funcional mal diret cadastr model exempl despach gq desp ice analis</t>
   </si>
   <si>
     <t>scann lig</t>
@@ -79,19 +79,19 @@
     <t>solicit auxili efetu limp scann</t>
   </si>
   <si>
-    <t>control extern si anális com dad colet tod anex process numer numer numer bimestr inform demonstr cl comprov envi dia numer solicit inform final inform</t>
-  </si>
-  <si>
-    <t>solicit cri míd extern process set</t>
+    <t>control extern si analis com dad colet tod anex process numer numer numer bimestr inform demonstr cl comprov envi dia numer solicit inform final inform</t>
+  </si>
+  <si>
+    <t>solicit cri mid extern process set</t>
   </si>
   <si>
     <t>serv consegu abr arqu pc</t>
   </si>
   <si>
-    <t>tent exclu transit process numer numer tc obedi rela event numer aparec seguint restr possível realiz exclus dest trânsit julg poi process relat possu dív pag</t>
-  </si>
-  <si>
-    <t>solicit seç sit apresent model vi vii si numer coloc descr model númer norm associ model vi códig receit orçamentár resoluç n numer numer tce port n numer numer gp tce model vii tabel padr códig font recurs resoluç n numer numer tce port n numer numer gp tce</t>
+    <t>tent exclu transit process numer numer tc obedi rela event numer aparec seguint restr possivel realiz exclus dest transit julg poi process relat possu div pag</t>
+  </si>
+  <si>
+    <t>solicit sec sit apresent model vi vii si numer coloc descr model numer norm associ model vi codig receit orcamentar resoluc n numer numer tce port n numer numer gp tce model vii tabel padr codig font recurs resoluc n numer numer tce port n numer numer gp tce</t>
   </si>
   <si>
     <t>al ter senh usu</t>
@@ -106,16 +106,16 @@
     <t>configur impres pc serv</t>
   </si>
   <si>
-    <t>retorn protest aleg outr jurisd endereç respons natal rn pro numer numer</t>
+    <t>retorn protest aleg outr jurisd enderec respons natal rn pro numer numer</t>
   </si>
   <si>
     <t>tend acess bi</t>
   </si>
   <si>
-    <t>solicit cancel trânsit julg process numer numer tc conform determin rela event numer</t>
-  </si>
-  <si>
-    <t>configur rádi plen pc serv</t>
+    <t>solicit cancel transit julg process numer numer tc conform determin rela event numer</t>
+  </si>
+  <si>
+    <t>configur radi plen pc serv</t>
   </si>
   <si>
     <t>al ter inform assin public</t>
@@ -130,10 +130,10 @@
     <t>solicit apoi operac edit inform process</t>
   </si>
   <si>
-    <t>bom dia solicit instal lrfserv produç instal fsdin dev instal serviç si lrfserv homolog obrig</t>
-  </si>
-  <si>
-    <t>usu solicit instal sql maquin uso diári</t>
+    <t>bom dia solicit instal lrfserv produc instal fsdin dev instal servic si lrfserv homolog obrig</t>
+  </si>
+  <si>
+    <t>usu solicit instal sql maquin uso diari</t>
   </si>
   <si>
     <t>apoi operac memor</t>
@@ -142,13 +142,13 @@
     <t>err inser inform</t>
   </si>
   <si>
-    <t>alt er senh áre restrit</t>
+    <t>alt er senh are restrit</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>cord cumpr ord procur geral solicit brev cas requ numer nobreak gabinet procur carl barr virtud quebr exist envi almoxarif constat diret informá</t>
+    <t>cord cumpr ord procur geral solicit brev cas requ numer nobreak gabinet procur carl barr virtud quebr exist envi almoxarif constat diret informa</t>
   </si>
   <si>
     <t>configur vpn notebook acess extern</t>
@@ -157,10 +157,10 @@
     <t>boa tard tent envi arqu ldo numer constat err aguard dev prossegu desd agrad ccedil</t>
   </si>
   <si>
-    <t>usuár solicit apoi operac uso equip</t>
-  </si>
-  <si>
-    <t>serv mp rn gaec veridian alv med port cpf numer matrícul numer numer email veridian alv mprn mp br solicit renov senh acess áre restrit tce</t>
+    <t>usuar solicit apoi operac uso equip</t>
+  </si>
+  <si>
+    <t>serv mp rn gaec veridian alv med port cpf numer matricul numer numer email veridian alv mprn mp br solicit renov senh acess are restrit tce</t>
   </si>
   <si>
     <t>verific err anex tent consult advog cadastr reprov port tce</t>
@@ -169,28 +169,28 @@
     <t>orient acerc pont</t>
   </si>
   <si>
-    <t>usuár solicit apoi aprov cadastr advog port tce</t>
-  </si>
-  <si>
-    <t>test relógi ref nf numer numer confer correspond especific envi propost fornec</t>
+    <t>usuar solicit apoi aprov cadastr advog port tce</t>
+  </si>
+  <si>
+    <t>test relogi ref nf numer numer confer correspond especific envi propost fornec</t>
   </si>
   <si>
     <t>valid document refer nf numer numer process numer numer</t>
   </si>
   <si>
-    <t>contat telefôn auxili usuár gerenci procurad geral est cadastr usu comum adicion permiss</t>
-  </si>
-  <si>
-    <t>cumpr estil venh solic constat err inclus inform exclus mesm seguint process execuç numer numer event numer numer numer event numer numer numer event numer numer numer event numer numer numer event numer</t>
-  </si>
-  <si>
-    <t>usuár solicit apoi operac digital document set solicit</t>
+    <t>contat telefon auxili usuar gerenci procurad geral est cadastr usu comum adicion permiss</t>
+  </si>
+  <si>
+    <t>cumpr estil venh solic constat err inclus inform exclus mesm seguint process execuc numer numer event numer numer numer event numer numer numer event numer numer numer event numer numer numer event numer</t>
+  </si>
+  <si>
+    <t>usuar solicit apoi operac digital document set solicit</t>
   </si>
   <si>
     <t>instal numer zip</t>
   </si>
   <si>
-    <t>usuár solicit técn acompanh equip extern event audit dat numer numer numer</t>
+    <t>usuar solicit tecn acompanh equip extern event audit dat numer numer numer</t>
   </si>
   <si>
     <t>usu solicit al ter senh email instituc</t>
@@ -199,13 +199,13 @@
     <t>tent consult legisl mei map sit tce rn aparec err anex</t>
   </si>
   <si>
-    <t>usuár solicit apoi operac uso arqu comput</t>
+    <t>usuar solicit apoi operac uso arqu comput</t>
   </si>
   <si>
     <t>solicit remanej comput</t>
   </si>
   <si>
-    <t>ord coorden geral solicit voss senh liber numer técn informá trabalh event crc conselh region contabil dia numer agost numer hor numeroh numeroh auditóri tce rn</t>
+    <t>ord coorden geral solicit voss senh liber numer tecn informa trabalh event crc conselh region contabil dia numer agost numer hor numeroh numeroh auditori tce rn</t>
   </si>
   <si>
     <t>liber pop up impress arqu</t>
@@ -217,13 +217,13 @@
     <t>verific comput lig restaurant</t>
   </si>
   <si>
-    <t>atend cham numer memor numer numer escol tal demand necess acess leit tabel anexonumer responsa ambi dev hom produç</t>
+    <t>atend cham numer memor numer numer escol tal demand necess acess leit tabel anexonumer responsa ambi dev hom produc</t>
   </si>
   <si>
     <t>configur scann</t>
   </si>
   <si>
-    <t>configur estaçã trabalh</t>
+    <t>configur estaca trabalh</t>
   </si>
   <si>
     <t>instal internet explor execut siaf</t>
@@ -235,7 +235,7 @@
     <t>instal softw pencil</t>
   </si>
   <si>
-    <t>proc numer numer volt cartóri sob aleg outr jurisd lig cartóri fal reenvi consig porqu aparec statu irregular proc numer numer volt cartóri sob aleg sust defini lig cartóri inform exist it sust lá pra estranh fal lá registr dat apresent inferi venc chamadonumer verific inconsist suger reenvi consig porqu statu irregular outr chamadonumer process</t>
+    <t>proc numer numer volt cartori sob aleg outr jurisd lig cartori fal reenvi consig porqu aparec statu irregular proc numer numer volt cartori sob aleg sust defini lig cartori inform exist it sust la pra estranh fal la registr dat apresent inferi venc chamadonumer verific inconsist suger reenvi consig porqu statu irregular outr chamadonumer process</t>
   </si>
   <si>
     <t>cadastr oper cpf numer nom ind cell xavi silv gom</t>
@@ -250,7 +250,7 @@
     <t>cadastr biometr</t>
   </si>
   <si>
-    <t>liber acess si anális legil</t>
+    <t>liber acess si analis legil</t>
   </si>
   <si>
     <t>emiss certific digit token</t>
@@ -259,73 +259,73 @@
     <t>cadastr oper cpf numer nom vit pimentel barb</t>
   </si>
   <si>
-    <t>acess cont gest companh águ esgot refer exercíci numer vári it numer numer numer numer numer numer aparec seguint mens err serv numer arqu diretóri encontr recurs procur pod ter sid remov ter tid nom alt er est tempor indispon</t>
-  </si>
-  <si>
-    <t>proc numer numer tent tramit acus aus public document vez permit public aparec símbol zer cort</t>
-  </si>
-  <si>
-    <t>venh através dest solic public sit tce dispon homolog fs lan appweb releas hom iissqlnumer wwwreleas</t>
-  </si>
-  <si>
-    <t>aprov solicit funcional códig numer nom fern antoni teix lea</t>
+    <t>acess cont gest companh agu esgot refer exercici numer vari it numer numer numer numer numer numer aparec seguint mens err serv numer arqu diretori encontr recurs procur pod ter sid remov ter tid nom alt er est tempor indispon</t>
+  </si>
+  <si>
+    <t>proc numer numer tent tramit acus aus public document vez permit public aparec simbol zer cort</t>
+  </si>
+  <si>
+    <t>venh atraves dest solic public sit tce dispon homolog fs lan appweb releas hom iissqlnumer wwwreleas</t>
+  </si>
+  <si>
+    <t>aprov solicit funcional codig numer nom fern antoni teix lea</t>
   </si>
   <si>
     <t>solicit estabiliz funcion impres nest set</t>
   </si>
   <si>
-    <t>usu solicit apoi operac áre infraestrut restaurant</t>
-  </si>
-  <si>
-    <t>numer cumpr estil venh solic adot med cab lot audi control extern ind cell xavi silv gom matrícul numer numer diret ato pessoal dap numer moment agradeç atenç destin solicit</t>
+    <t>usu solicit apoi operac are infraestrut restaurant</t>
+  </si>
+  <si>
+    <t>numer cumpr estil venh solic adot med cab lot audi control extern ind cell xavi silv gom matricul numer numer diret ato pessoal dap numer moment agradec atenc destin solicit</t>
   </si>
   <si>
     <t>cumpr estil solicit levant banc dad list process tip process alt er bge lrf fqm rel bge ppa ldo orc tip apr apur respons</t>
   </si>
   <si>
-    <t>solicit auxíli substitu inform process</t>
-  </si>
-  <si>
-    <t>ord procur geral minist públic cont thiag martim guterr venh solic acess serv leandr ces cruz sá lorenzett págin áre restrit vincul procurad geral sob seguint denomin proc prest cont</t>
-  </si>
-  <si>
-    <t>solicit realiz pesquis preç merc mater relacion memor numer numer din sup</t>
-  </si>
-  <si>
-    <t>cumpr solicit exclu pend monitor red hospital emiss cert prefeit mossoró refer audit operac realiz red hospital est consider relatóri audit emit</t>
-  </si>
-  <si>
-    <t>vim intermédi pres instrument report algum inconsist prop algum sugest melhor formul gerenci inscr estagi conform relaç abaix numer inconsist deix nom pai branc ger imprim formul camp vem preench nom harold fernand duart juni ana cláud b sistem traz dad secret geral gest anteri c camp mail send preench val difer preench numer sugest cri espéci common box camp pai mãe opç inform b cri opç permit usu cadastr alt er camp refer dad secret geral vir pré preench moment cadastr nov estagi c usu inform institu ensin camp vir pre preench d cri camp nom crach</t>
-  </si>
-  <si>
-    <t>cumpr estil solicit baix atend intim n numer numer dae dev requer sr antôni walt er araúj</t>
-  </si>
-  <si>
-    <t>aprov solicit funcional códig numer nom tiag tomaz cost silv</t>
+    <t>solicit auxili substitu inform process</t>
+  </si>
+  <si>
+    <t>ord procur geral minist public cont thiag martim guterr venh solic acess serv leandr ces cruz sa lorenzett pagin are restrit vincul procurad geral sob seguint denomin proc prest cont</t>
+  </si>
+  <si>
+    <t>solicit realiz pesquis prec merc mater relacion memor numer numer din sup</t>
+  </si>
+  <si>
+    <t>cumpr solicit exclu pend monitor red hospital emiss cert prefeit mossoro refer audit operac realiz red hospital est consider relatori audit emit</t>
+  </si>
+  <si>
+    <t>vim intermedi pres instrument report algum inconsist prop algum sugest melhor formul gerenci inscr estagi conform relac abaix numer inconsist deix nom pai branc ger imprim formul camp vem preench nom harold fernand duart juni ana claud b sistem traz dad secret geral gest anteri c camp mail send preench val difer preench numer sugest cri especi common box camp pai mae opc inform b cri opc permit usu cadastr alt er camp refer dad secret geral vir pre preench moment cadastr nov estagi c usu inform institu ensin camp vir pre preench d cri camp nom crach</t>
+  </si>
+  <si>
+    <t>cumpr estil solicit baix atend intim n numer numer dae dev requer sr antoni walt er arauj</t>
+  </si>
+  <si>
+    <t>aprov solicit funcional codig numer nom tiag tomaz cost silv</t>
   </si>
   <si>
     <t>acess past dap dap ben</t>
   </si>
   <si>
-    <t>venh através dest solic public sistem port ges ja dispon homolog fs lan appweb hom hom iissqlnumer portalgestorhom substitu past config</t>
-  </si>
-  <si>
-    <t>alt eraç proced banc respons cri remess xml protest</t>
+    <t>venh atraves dest solic public sistem port ges ja dispon homolog fs lan appweb hom hom iissqlnumer portalgestorhom substitu past config</t>
+  </si>
+  <si>
+    <t>alt erac proced banc respons cri remess xml protest</t>
   </si>
   <si>
     <t>alt ere senh serv aposent francisc assil per cpf numer</t>
   </si>
   <si>
-    <t>tent efetu registr ato process list set págin apresent mens const anex</t>
-  </si>
-  <si>
-    <t>bom dia suport técn empr softw agil rn detect problem anex numer receit ond relatóri si invé deduz val receit ind tip numer deduç fundeb som ocasion assim diverg seg anex document detalh problem arqu backupsi lrf arqu txt anális respec inform ob test feit numerobim vist ocorr tod demal grat desd inform fic aguard retorn</t>
-  </si>
-  <si>
-    <t>detect dív sistem process cit comarc cit n numer cuj municípi cit exist tabel comarc homolog protest</t>
-  </si>
-  <si>
-    <t>detect pesso sistem process cit comarc pesso id numer cuj municípi residenc exist tabel comarc homolog protest</t>
+    <t>tent efetu registr ato process list set pagin apresent mens const anex</t>
+  </si>
+  <si>
+    <t>bom dia suport tecn empr softw agil rn detect problem anex numer receit ond relatori si inve deduz val receit ind tip numer deduc fundeb som ocasion assim diverg seg anex document detalh problem arqu backupsi lrf arqu txt analis respec inform ob test feit numerobim vist ocorr tod demal grat desd inform fic aguard retorn</t>
+  </si>
+  <si>
+    <t>detect div sistem process cit comarc cit n numer cuj municipi cit exist tabel comarc homolog protest</t>
+  </si>
+  <si>
+    <t>detect pesso sistem process cit comarc pesso id numer cuj municipi residenc exist tabel comarc homolog protest</t>
   </si>
   <si>
     <t>detect registr tabel exe debit possu decis relacion possu camp idinformaca preench pod ger registr problem futur protest idcomposicaopautanumer</t>
@@ -346,25 +346,25 @@
     <t>renov certific digit bi tce rn gov br</t>
   </si>
   <si>
-    <t>err funcional áre restrit</t>
+    <t>err funcional are restrit</t>
   </si>
   <si>
     <t>inclu tip conveni tip serv</t>
   </si>
   <si>
-    <t>consig ger decis monocrá sistem reincid abert cham anteri sobr assunt aus tip registr registr ressalv registr process numer numer tc aguard respost</t>
+    <t>consig ger decis monocra sistem reincid abert cham anteri sobr assunt aus tip registr registr ressalv registr process numer numer tc aguard respost</t>
   </si>
   <si>
     <t>al ter avali pont dire substitut infocex</t>
   </si>
   <si>
-    <t>usuár solicit suport abr arqu consult médic</t>
+    <t>usuar solicit suport abr arqu consult medic</t>
   </si>
   <si>
     <t>solicit acess emiss certific dentr aba administr escol cont</t>
   </si>
   <si>
-    <t>implement págin cadastr institu ensin cadastr estági</t>
+    <t>implement pagin cadastr institu ensin cadastr estagi</t>
   </si>
   <si>
     <t>identific numer registr anex numer desp duplic process inform terc bimestr prefeit camp grand seg planilh anex inform duplic grif amarel</t>
@@ -373,19 +373,19 @@
     <t>mens err detalh impossibilit acess program</t>
   </si>
   <si>
-    <t>ord coorden geral solicit voss senh liber numer técn informá trabalh event audi técn mudanç si exercíci numer dia numer numer numer hor numeroh numeroh auditóri tce rn</t>
+    <t>ord coorden geral solicit voss senh liber numer tecn informa trabalh event audi tecn mudanc si exercici numer dia numer numer numer hor numeroh numeroh auditori tce rn</t>
   </si>
   <si>
     <t>ord exm sr procur luci silv cost ram venh solic din inici proced necess renov certific digit procur cuj venc ocorr dat hoj</t>
   </si>
   <si>
-    <t>cord cumpr solicit adequ relatóri cont opç relatori process process registr deneg dev cont seguint ajust numer possibil filtr event açã coorden numer possibil visual númer process list numer correç relatóri vind vazi numer relatóri dev cont mesm colun list orig consider realiz reun prév serv thiag hudson solicit encaminh demand cient atend pleit agradec desd atenç dispens</t>
-  </si>
-  <si>
-    <t>cord saud solicit revis relatóri produt local opç relatori resum gerenc produt set usu it relat anális process cient atend pleit agradec desd atenç confer demand</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom erik alexandr gom</t>
+    <t>cord cumpr solicit adequ relatori cont opc relatori process process registr deneg dev cont seguint ajust numer possibil filtr event aca coorden numer possibil visual numer process list numer correc relatori vind vazi numer relatori dev cont mesm colun list orig consider realiz reun prev serv thiag hudson solicit encaminh demand cient atend pleit agradec desd atenc dispens</t>
+  </si>
+  <si>
+    <t>cord saud solicit revis relatori produt local opc relatori resum gerenc produt set usu it relat analis process cient atend pleit agradec desd atenc confer demand</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom erik alexandr gom</t>
   </si>
   <si>
     <t>prepar pc proje sal reun presid</t>
@@ -400,25 +400,25 @@
     <t>conced permiss admin local pc</t>
   </si>
   <si>
-    <t>prez solicit determin procur ricart cés coelh sant providenc export míd eletrôn refer process n numer numer tc esclareç oportun míd pod ser disponibil através past públic dest gabinet srv fsnumer publ proc gab ricart atencios múci med numer numer</t>
+    <t>prez solicit determin procur ricart ces coelh sant providenc export mid eletron refer process n numer numer tc esclarec oportun mid pod ser disponibil atraves past public dest gabinet srv fsnumer publ proc gab ricart atencios muci med numer numer</t>
   </si>
   <si>
     <t>apoi operac abr arqu</t>
   </si>
   <si>
-    <t>alt eraç oper cpf numer nom dhyog tav silv moral</t>
+    <t>alt erac oper cpf numer nom dhyog tav silv moral</t>
   </si>
   <si>
     <t>configur oper</t>
   </si>
   <si>
-    <t>possível conclu cadastr falt cóp ato nome carg ocup órg gerent control preven conform previst port n numer numer tc</t>
-  </si>
-  <si>
-    <t>ord coorden geral solicit voss senh autor reserv auditóri tce demal provid realiz event audi técn mudanç si exercíci numer dia numer numer numer hor numeroh numeroh reserv auditóri tce rn design técn manutenç sonor ar condicion assessor equip escol cont dur event equp realiz limp auditóri banh vésp dur hor event</t>
-  </si>
-  <si>
-    <t>possível conclu cadastr falt port design usu gerenci conform previst port n numer numer tc</t>
+    <t>possivel conclu cadastr falt cop ato nome carg ocup org gerent control preven conform previst port n numer numer tc</t>
+  </si>
+  <si>
+    <t>ord coorden geral solicit voss senh autor reserv auditori tce demal provid realiz event audi tecn mudanc si exercici numer dia numer numer numer hor numeroh numeroh reserv auditori tce rn design tecn manutenc sonor ar condicion assessor equip escol cont dur event equp realiz limp auditori banh vesp dur hor event</t>
+  </si>
+  <si>
+    <t>possivel conclu cadastr falt port design usu gerenci conform previst port n numer numer tc</t>
   </si>
   <si>
     <t>inclu grup acess cpd dev admin ad</t>
@@ -427,13 +427,13 @@
     <t>cadastr usu gerenci</t>
   </si>
   <si>
-    <t>alt eraç oper cpf numer nom rafael dia sant</t>
-  </si>
-  <si>
-    <t>venh solic gentil alt eraç títul últ notíc inser mes notíc aba ouvid http www tce rn gov br ouvid mesadenotic tce fec realiz capacit câm municip jardim seridó dev ser profiss contabil natal discut sobr import control soc est algum motiv consegu faz alt eraç coment ferrament eletrôn áre restrit denomin cadastr págin set poi clic naquel ícon amarel ediç nad aparec apen notíc consig edit tod outr</t>
-  </si>
-  <si>
-    <t>consider advent lei complement n numer numer mai numer ond extingu secret est justiç cidadan sejuc cri secret est administr penitenciár seap serv pres solic esclarec relaç cont gest exercíci numer secret est justiç cidadan especific relaç cont jan mai exercíci numer</t>
+    <t>alt erac oper cpf numer nom rafael dia sant</t>
+  </si>
+  <si>
+    <t>venh solic gentil alt erac titul ult notic inser mes notic aba ouvid http www tce rn gov br ouvid mesadenotic tce fec realiz capacit cam municip jardim serido dev ser profiss contabil natal discut sobr import control soc est algum motiv consegu faz alt erac coment ferrament eletron are restrit denomin cadastr pagin set poi clic naquel icon amarel edic nad aparec apen notic consig edit tod outr</t>
+  </si>
+  <si>
+    <t>consider advent lei complement n numer numer mai numer ond extingu secret est justic cidadan sejuc cri secret est administr penitenciar seap serv pres solic esclarec relac cont gest exercici numer secret est justic cidadan especific relac cont jan mai exercici numer</t>
   </si>
   <si>
     <t>apoi operac cancel envi public din</t>
@@ -442,115 +442,115 @@
     <t>atualiz versa numer tent ger numer bim pod ver resolv problem siop est dand tel err</t>
   </si>
   <si>
-    <t>receb mail procurad geral justiç pergunt sobr sispatr cas serv efet deslig funç gratific institu permanec norm carg efet di diss pergunt necess envi declar said refer apen funç gratific respond precis declar</t>
-  </si>
-  <si>
-    <t>receb lig ped orient sab praz process envi pet inic encaminh protocol inic presenc acompanh and através port tec</t>
-  </si>
-  <si>
-    <t>aprov solicit funcional códig numer nom shár so jewur</t>
-  </si>
-  <si>
-    <t>cadastr ocorrenc hardw problem encontr comput posi dnumer defeit entr sistem problem hd tomb numer usu kalin set recepç problem detect</t>
-  </si>
-  <si>
-    <t>cumpr estil solicit acess serv eric kaline barb souz brit sal arauj matrícul numer numer cpf numer set dam coorden fiscal cont govern através áre restrit past compartilh dam fgo srv fsnumer dam fgo</t>
-  </si>
-  <si>
-    <t>cumpr estil solicit cadastr estagiár ana beatriz so macêd cpf numer numer numer áre restrit tce rn vincul perfil coorden fiscal cont govern dam fgo cadastr biometr acess sistem control pont oportun solicit aind conced perfil acess funcional atribu estagiár rafael rib cabr matrícul numer cpf numer</t>
+    <t>receb mail procurad geral justic pergunt sobr sispatr cas serv efet deslig func gratific institu permanec norm carg efet di diss pergunt necess envi declar said refer apen func gratific respond precis declar</t>
+  </si>
+  <si>
+    <t>receb lig ped orient sab praz process envi pet inic encaminh protocol inic presenc acompanh and atraves port tec</t>
+  </si>
+  <si>
+    <t>aprov solicit funcional codig numer nom shar so jewur</t>
+  </si>
+  <si>
+    <t>cadastr ocorrenc hardw problem encontr comput posi dnumer defeit entr sistem problem hd tomb numer usu kalin set recepc problem detect</t>
+  </si>
+  <si>
+    <t>cumpr estil solicit acess serv eric kaline barb souz brit sal arauj matricul numer numer cpf numer set dam coorden fiscal cont govern atraves are restrit past compartilh dam fgo srv fsnumer dam fgo</t>
+  </si>
+  <si>
+    <t>cumpr estil solicit cadastr estagiar ana beatriz so maced cpf numer numer numer are restrit tce rn vincul perfil coorden fiscal cont govern dam fgo cadastr biometr acess sistem control pont oportun solicit aind conced perfil acess funcional atribu estagiar rafael rib cabr matricul numer cpf numer</t>
   </si>
   <si>
     <t>solicit apoi operac celul</t>
   </si>
   <si>
-    <t>alt eraç oper cpf numer nom ind cell xavi silv gom</t>
+    <t>alt erac oper cpf numer nom ind cell xavi silv gom</t>
   </si>
   <si>
     <t>solicit apoi operac assin inform</t>
   </si>
   <si>
-    <t>aparec consult diári ofic compreend períod numer numer numer numer numer numer</t>
+    <t>aparec consult diari ofic compreend period numer numer numer numer numer numer</t>
   </si>
   <si>
     <t>orient acess sit instituc hom offic</t>
   </si>
   <si>
-    <t>process numer numer volt protest irregular tent reenvi aparec imped aparec págin permit envi</t>
-  </si>
-  <si>
-    <t>cumpr estil solicit acess serv anderson josé nasc lim matrícul numer numer cpf numer glac silv august pimentel matrícul numer numer cpf numer set dam coorden fiscal cont gest através áre restrit past compartilh dam fge srv fsnumer dam fge</t>
-  </si>
-  <si>
-    <t>cord cumpr ord dire informá particip fornec daysian gom david solicit dil praz entreg refer ord compr numer numer not empenh numer numer anex relat aquis numer quatr caix acús ser instal plen dinart mariz conform mail envi fornec aleg temporár indisponibil matér prim fabric caix acús solicit dat máx entreg inic apraz numer numer numer prorrog numer trint dia numer numer numer</t>
-  </si>
-  <si>
-    <t>senh dire cient determin impost cort cont espec cont control relacion seguranç comun v sa exclus serv renat freit silv cpf numer tod sistem tce rn part dia numer numer numer términ ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informá provid cab</t>
-  </si>
-  <si>
-    <t>bom dia solicit public siaianaliseap siaianalis produç sistem encontr homolog obrig</t>
-  </si>
-  <si>
-    <t>retific si prefeit caiç rio vent numer numer bimestr si pq diverg receit siop envi numer bimestr apresent seguint err conform anex entant val pag rcifra numer numer conform err bimestr anteri refer projet ativ numer ensin fundament val pag bimestr atual val rcifra numer numer refer projet ativ porém educ infantil ent ent pod dand crít process respost solicit atualiz si vers disponibil sit n numer segu ger arqu prest cont nov segu surgir mens err dev alt eraç ser realiz registr receit conform seg anex</t>
-  </si>
-  <si>
-    <t>cumpr estil venh mei dest expedi solic conform acord reun dia numer numer numer sal infocex acess bas dad sistem channel através usu perfil consult via metabas sql serv management studi objetiv desenvolv painel acompanh execuç plan fiscal anual pfa</t>
+    <t>process numer numer volt protest irregular tent reenvi aparec imped aparec pagin permit envi</t>
+  </si>
+  <si>
+    <t>cumpr estil solicit acess serv anderson jose nasc lim matricul numer numer cpf numer glac silv august pimentel matricul numer numer cpf numer set dam coorden fiscal cont gest atraves are restrit past compartilh dam fge srv fsnumer dam fge</t>
+  </si>
+  <si>
+    <t>cord cumpr ord dire informa particip fornec daysian gom david solicit dil praz entreg refer ord compr numer numer not empenh numer numer anex relat aquis numer quatr caix acus ser instal plen dinart mariz conform mail envi fornec aleg temporar indisponibil mater prim fabric caix acus solicit dat max entreg inic apraz numer numer numer prorrog numer trint dia numer numer numer</t>
+  </si>
+  <si>
+    <t>senh dire cient determin impost cort cont espec cont control relacion seguranc comun v sa exclus serv renat freit silv cpf numer tod sistem tce rn part dia numer numer numer termin ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informa provid cab</t>
+  </si>
+  <si>
+    <t>bom dia solicit public siaianaliseap siaianalis produc sistem encontr homolog obrig</t>
+  </si>
+  <si>
+    <t>retific si prefeit caic rio vent numer numer bimestr si pq diverg receit siop envi numer bimestr apresent seguint err conform anex entant val pag rcifra numer numer conform err bimestr anteri refer projet ativ numer ensin fundament val pag bimestr atual val rcifra numer numer refer projet ativ porem educ infantil ent ent pod dand crit process respost solicit atualiz si vers disponibil sit n numer segu ger arqu prest cont nov segu surgir mens err dev alt erac ser realiz registr receit conform seg anex</t>
+  </si>
+  <si>
+    <t>cumpr estil venh mei dest expedi solic conform acord reun dia numer numer numer sal infocex acess bas dad sistem channel atraves usu perfil consult via metabas sql serv management studi objetiv desenvolv painel acompanh execuc plan fiscal anual pfa</t>
   </si>
   <si>
     <t>solicit apoi operac local arqu process</t>
   </si>
   <si>
-    <t>verific process numer numer usu quer visual document inform aind public assin sistem retorn mens possível encontr arqu usu inform pod exclu inform poi sab inform necessár</t>
-  </si>
-  <si>
-    <t>solicit cri cham abert recorr seman sext feir numeroh seguint descr realiz manutenç preven scann instal diret expedi inclu limp intern remoç possível objet estranh poss danific equip coloc joã mar respons rutêni atend michely solicit</t>
-  </si>
-  <si>
-    <t>realiz manutenç preven scann instal diret expedi inclu limp intern remoç possível objet estranh poss danific equip</t>
-  </si>
-  <si>
-    <t>venh através dest solic acess usu usit leit tabel bdsi dbo anexonumer pessoaucc ambi dev homolog produç</t>
+    <t>verific process numer numer usu quer visual document inform aind public assin sistem retorn mens possivel encontr arqu usu inform pod exclu inform poi sab inform necessar</t>
+  </si>
+  <si>
+    <t>solicit cri cham abert recorr seman sext feir numeroh seguint descr realiz manutenc preven scann instal diret expedi inclu limp intern remoc possivel objet estranh poss danific equip coloc joa mar respons ruteni atend michely solicit</t>
+  </si>
+  <si>
+    <t>realiz manutenc preven scann instal diret expedi inclu limp intern remoc possivel objet estranh poss danific equip</t>
+  </si>
+  <si>
+    <t>venh atraves dest solic acess usu usit leit tabel bdsi dbo anexonumer pessoaucc ambi dev homolog produc</t>
   </si>
   <si>
     <t>orient sobr sess ativ pc envi memor</t>
   </si>
   <si>
-    <t>ofert cumpr estil ord procur luci rib camp envi mei dest memor rubr solicit diret informá t i marcel elabor relatóri receit anteri solicit gabinet atencios</t>
-  </si>
-  <si>
-    <t>tent cadastr requer func tip adic titul opç anex arqu desaparec tel tão log escolh tip requer func observ tel inic capturarnumer mesm tel após escolh tip requer capturarnumer solicit mant opç anex arqu após escolh tip requer</t>
-  </si>
-  <si>
-    <t>cadastr oper cpf numer nom vit hug araúj pint</t>
-  </si>
-  <si>
-    <t>venh através dest solic public sit tce dispon homolog</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom viníc josé mirand tosc brit filh</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom andré gustav alme silv</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom dav rib cunh</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom rutêni sampai pásco</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom ana keil dant araúj queiroz</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom walt er mous mor júni</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom felip barb nicolau fernand</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom jos alex sous</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom andré boratt torquat</t>
+    <t>ofert cumpr estil ord procur luci rib camp envi mei dest memor rubr solicit diret informa t i marcel elabor relatori receit anteri solicit gabinet atencios</t>
+  </si>
+  <si>
+    <t>tent cadastr requer func tip adic titul opc anex arqu desaparec tel tao log escolh tip requer func observ tel inic capturarnumer mesm tel apos escolh tip requer capturarnumer solicit mant opc anex arqu apos escolh tip requer</t>
+  </si>
+  <si>
+    <t>cadastr oper cpf numer nom vit hug arauj pint</t>
+  </si>
+  <si>
+    <t>venh atraves dest solic public sit tce dispon homolog</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom vinic jose mirand tosc brit filh</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom andre gustav alme silv</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom dav rib cunh</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom ruteni sampai pasco</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom ana keil dant arauj queiroz</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom walt er mous mor juni</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom felip barb nicolau fernand</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom jos alex sous</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom andre boratt torquat</t>
   </si>
   <si>
     <t>ad conced acess past glob dap</t>
@@ -559,13 +559,13 @@
     <t>usu aleg comput red</t>
   </si>
   <si>
-    <t>configur áre trabalh</t>
+    <t>configur are trabalh</t>
   </si>
   <si>
     <t>ofert cumpr estil anex memor arqu word dad prev solicit ti marcel</t>
   </si>
   <si>
-    <t>numer cumpr estil solicit ger arqu cont extr atual dad si fiscal compartilh dest políci civil minist públic est atend acord cooper técn firm cort cont numer vez ger supracit arqu favor inform link ser utiliz download institu parc epígraf numer moment coloc dispos demal esclarec</t>
+    <t>numer cumpr estil solicit ger arqu cont extr atual dad si fiscal compartilh dest polici civil minist public est atend acord cooper tecn firm cort cont numer vez ger supracit arqu favor inform link ser utiliz download institu parc epigraf numer moment coloc dispos demal esclarec</t>
   </si>
   <si>
     <t>solicit configur impres pc</t>
@@ -580,13 +580,13 @@
     <t>configur tecl</t>
   </si>
   <si>
-    <t>cadastr oper cpf numer nom ana beatriz so macêd</t>
+    <t>cadastr oper cpf numer nom ana beatriz so maced</t>
   </si>
   <si>
     <t>pc lig</t>
   </si>
   <si>
-    <t>realiz cadastr biometr estagiár</t>
+    <t>realiz cadastr biometr estagiar</t>
   </si>
   <si>
     <t>realiz cadastr biometr estagi</t>
@@ -598,19 +598,19 @@
     <t>solicit configur internet celul</t>
   </si>
   <si>
-    <t>relat nobreak tce patr numer tce numer local set suport apresent falh carg conseg desempenh ativ diár</t>
+    <t>relat nobreak tce patr numer tce numer local set suport apresent falh carg conseg desempenh ativ diar</t>
   </si>
   <si>
     <t>configur internet celul</t>
   </si>
   <si>
-    <t>aprov solicit funcional códig numer nom ind cell xavi silv gom</t>
+    <t>aprov solicit funcional codig numer nom ind cell xavi silv gom</t>
   </si>
   <si>
     <t>solicit configur moni secund</t>
   </si>
   <si>
-    <t>solicit substitu equip informá numer nobreak numer estabiliz defeit numer doi nobreak nov</t>
+    <t>solicit substitu equip informa numer nobreak numer estabiliz defeit numer doi nobreak nov</t>
   </si>
   <si>
     <t>instal ergon</t>
@@ -622,10 +622,10 @@
     <t>aprov cadastr advog port tce sistem inform ok entant nom requer realiz registr deix solicit tel</t>
   </si>
   <si>
-    <t>usu solicit apoi efetu requer justific pont áre restrit</t>
-  </si>
-  <si>
-    <t>prez coorden com cumpriment estil solicit liber acess serv jadson anderson med silv víde aul dispon youtub virtud matrícul curs ead necess visual refer aul refer curs audit base risc disponibil tcu cuj inscr ampl foment escol cont dest tribun</t>
+    <t>usu solicit apoi efetu requer justific pont are restrit</t>
+  </si>
+  <si>
+    <t>prez coorden com cumpriment estil solicit liber acess serv jadson anderson med silv vide aul dispon youtub virtud matricul curs ead necess visual refer aul refer curs audit base risc disponibil tcu cuj inscr ampl foment escol cont dest tribun</t>
   </si>
   <si>
     <t>realiz avali carg si n numer pmparnam mesm falh carg</t>
@@ -637,40 +637,40 @@
     <t>apoi operac acess sistem</t>
   </si>
   <si>
-    <t>alt eraç oper cpf numer nom mari bezerr ferr</t>
+    <t>alt erac oper cpf numer nom mari bezerr ferr</t>
   </si>
   <si>
     <t>seg err process port ges refer numer bimestr pm rafael fernand</t>
   </si>
   <si>
-    <t>venh através dest solic public sistem siaianalis client siaianalis api mesm dispon homolog fs lan appweb hom</t>
-  </si>
-  <si>
-    <t>gost sab edit outr municípi port licit fácil jucurutu encontr respost prez realiz busc process licitatóri prefeit municip jucurutu através sit licit fácil identific registr envi conform print anex dess form gostari esclarec problem algum process licitatóri especifici qualqu dúv dispos</t>
+    <t>venh atraves dest solic public sistem siaianalis client siaianalis api mesm dispon homolog fs lan appweb hom</t>
+  </si>
+  <si>
+    <t>gost sab edit outr municipi port licit facil jucurutu encontr respost prez realiz busc process licitatori prefeit municip jucurutu atraves sit licit facil identific registr envi conform print anex dess form gostari esclarec problem algum process licitatori especifici qualqu duv dispos</t>
   </si>
   <si>
     <t>atual chrom</t>
   </si>
   <si>
-    <t>apoi cri model inform áre restrit</t>
-  </si>
-  <si>
-    <t>possível conclu cadastr dev falt port design usu gerenci acord port n numer numer tc</t>
-  </si>
-  <si>
-    <t>serv gabriel dia consegu acess áre restrit aqu dap</t>
-  </si>
-  <si>
-    <t>áre restrit necessit configur</t>
-  </si>
-  <si>
-    <t>venh através dest solic public sistem sispatr sispatrihom encontr homolog</t>
-  </si>
-  <si>
-    <t>configur comput nov estagiár</t>
-  </si>
-  <si>
-    <t>nov funcional inclu process paut dev aparec soment relatóri vot vot integr</t>
+    <t>apoi cri model inform are restrit</t>
+  </si>
+  <si>
+    <t>possivel conclu cadastr dev falt port design usu gerenci acord port n numer numer tc</t>
+  </si>
+  <si>
+    <t>serv gabriel dia consegu acess are restrit aqu dap</t>
+  </si>
+  <si>
+    <t>are restrit necessit configur</t>
+  </si>
+  <si>
+    <t>venh atraves dest solic public sistem sispatr sispatrihom encontr homolog</t>
+  </si>
+  <si>
+    <t>configur comput nov estagiar</t>
+  </si>
+  <si>
+    <t>nov funcional inclu process paut dev aparec soment relatori vot vot integr</t>
   </si>
   <si>
     <t>nov funcional inclu process paut selec inform prim process indic replic outr process funcional dev encontr inform correlacion cad process aliment camp corp instru</t>
@@ -679,25 +679,25 @@
     <t>orient reinici pc</t>
   </si>
   <si>
-    <t>solicit public lrfserviç produç instal fsdin dev instal serviç si lrfserv homolog obrig</t>
-  </si>
-  <si>
-    <t>program gerenc adob creativ cloud apresent err reinici efetu loff cont cadastr pass usu senh precis feit login nov possível ver solicit memor numer numer dia numer numer sobr inform relat quest usu cont adob</t>
+    <t>solicit public lrfservic produc instal fsdin dev instal servic si lrfserv homolog obrig</t>
+  </si>
+  <si>
+    <t>program gerenc adob creativ cloud apresent err reinici efetu loff cont cadastr pass usu senh precis feit login nov possivel ver solicit memor numer numer dia numer numer sobr inform relat quest usu cont adob</t>
   </si>
   <si>
     <t>apoi operac token desbloquei</t>
   </si>
   <si>
-    <t>usuár solicit apoi verific red comput</t>
-  </si>
-  <si>
-    <t>cord cumpr consequ reun realiz dia numer agost dest ano correged tce rn junt set envolv açã coorden ato pessoal equip corre dap sess din dae sirv pres expedi solic seguint melh áre restrit fim execuç açã coorden segu descrit numer indic funcional process set process possu pesso interess numer construç filtr list apen process possu pesso interess numer inclus tr tramit process possu pesso interess numer cri justific sistem pont efeit semelh sistem férias açã coorden moment renov vot est consider</t>
+    <t>usuar solicit apoi verific red comput</t>
+  </si>
+  <si>
+    <t>cord cumpr consequ reun realiz dia numer agost dest ano correged tce rn junt set envolv aca coorden ato pessoal equip corre dap sess din dae sirv pres expedi solic seguint melh are restrit fim execuc aca coorden segu descrit numer indic funcional process set process possu pesso interess numer construc filtr list apen process possu pesso interess numer inclus tr tramit process possu pesso interess numer cri justific sistem pont efeit semelh sistem ferias aca coorden moment renov vot est consider</t>
   </si>
   <si>
     <t>sirv pres cumpr estil solic renov certific digit serv camil germ queiroz saldanh</t>
   </si>
   <si>
-    <t>solicit public tceadmin produç aplic encontr homolog obrig</t>
+    <t>solicit public tceadmin produc aplic encontr homolog obrig</t>
   </si>
   <si>
     <t>procur relat tend problem assin inform process sele numer numer</t>
@@ -706,7 +706,7 @@
     <t>seg anex</t>
   </si>
   <si>
-    <t>venh através dest solic public sistem siaianalis especific arqu fs lan appweb hom hom iissqlnumer siaianalisehom app si analis anexonumer anexonumer singl anexonumer singl component html</t>
+    <t>venh atraves dest solic public sistem siaianalis especific arqu fs lan appweb hom hom iissqlnumer siaianalisehom app si analis anexonumer anexonumer singl anexonumer singl component html</t>
   </si>
   <si>
     <t>apoi operac instal program</t>
@@ -715,7 +715,7 @@
     <t>realiz avali retorn bolet n numer falh carg</t>
   </si>
   <si>
-    <t>cord cumpr ord dire informá refer ord compr numer numer empenh numer numer submet solicit prorrog praz entreg emit empr daysian gom david apreci deliber sr secret administr geral dest tribun cont</t>
+    <t>cord cumpr ord dire informa refer ord compr numer numer empenh numer numer submet solicit prorrog praz entreg emit empr daysian gom david apreci deliber sr secret administr geral dest tribun cont</t>
   </si>
   <si>
     <t>realiz verific upload cas necess ar fisic past ar digit</t>
@@ -730,7 +730,7 @@
     <t>usu gost sab proced pra cadastr usu gerenci inform necess solic cadastr via sit tribun segu parametr port numer numer</t>
   </si>
   <si>
-    <t>usu inform faz part associ fim lucr entr contat fim peg cert nega associ inform port ges possível retir cert nega apen órg jurisdicion pesso fisic encaminh ja outr tip cert emit lá</t>
+    <t>usu inform faz part associ fim lucr entr contat fim peg cert nega associ inform port ges possivel retir cert nega apen org jurisdicion pesso fisic encaminh ja outr tip cert emit la</t>
   </si>
   <si>
     <t>suport siab</t>
@@ -748,10 +748,10 @@
     <t>apoi operac digital document</t>
   </si>
   <si>
-    <t>apoi operac monocrá</t>
-  </si>
-  <si>
-    <t>realiz ajust págin inic transpar jurisdicion conform document anex ob numer link observatóri dev apont painel bi send constru numer link consult detalh dev apont consult órg utiliz hoj http www tce rn gov br transparenciajurisdicion consultaorga numer link dad abert dev apont funcional exist http apidadosabert tce rn gov br</t>
+    <t>apoi operac monocra</t>
+  </si>
+  <si>
+    <t>realiz ajust pagin inic transpar jurisdicion conform document anex ob numer link observatori dev apont painel bi send constru numer link consult detalh dev apont consult org utiliz hoj http www tce rn gov br transparenciajurisdicion consultaorga numer link dad abert dev apont funcional exist http apidadosabert tce rn gov br</t>
   </si>
   <si>
     <t>configur videoconfer</t>
@@ -769,16 +769,16 @@
     <t>problem ton</t>
   </si>
   <si>
-    <t>al dat public d decis monocrá pud faz registr ato</t>
+    <t>al dat public d decis monocra pud faz registr ato</t>
   </si>
   <si>
     <t>problem apens process</t>
   </si>
   <si>
-    <t>possível conclu cadastr falt port design usu gerenci conform port n numer numer tc</t>
-  </si>
-  <si>
-    <t>verific açã upload págin ferrament sit cadastr arqu sit verific págin set arqu local err local err arquivossit planejamentoestrateg local corret arquivossit download planejamentoestrateg</t>
+    <t>possivel conclu cadastr falt port design usu gerenci conform port n numer numer tc</t>
+  </si>
+  <si>
+    <t>verific aca upload pagin ferrament sit cadastr arqu sit verific pagin set arqu local err local err arquivossit planejamentoestrateg local corret arquivossit download planejamentoestrateg</t>
   </si>
   <si>
     <t>instal icpbrav</t>
@@ -793,10 +793,10 @@
     <t>substitu mous problem pc posi nov</t>
   </si>
   <si>
-    <t>aprov solicit funcional códig numer nom isold mar cost per</t>
-  </si>
-  <si>
-    <t>anex numer companh águ esgot rn caern setembr um val alt diz objet abr edit abaix relacion val númer recib recib numer rcifra numer numer numer recib numer rcifra numer numer numer recib numer rcifra numer numer numer</t>
+    <t>aprov solicit funcional codig numer nom isold mar cost per</t>
+  </si>
+  <si>
+    <t>anex numer companh agu esgot rn caern setembr um val alt diz objet abr edit abaix relacion val numer recib recib numer rcifra numer numer numer recib numer rcifra numer numer numer recib numer rcifra numer numer numer</t>
   </si>
   <si>
     <t>process numer numer deu problem assinat aparec seguint mens inform pend assinat digit set dae sei contat resolv pend</t>
@@ -811,19 +811,19 @@
     <t>solicit instal ergon past dap dap ben icpbrav ergon</t>
   </si>
   <si>
-    <t>prez bom dia acontec mens tant aba adit execuç prest cont dev proced grat vez ajud respost ant inser dad camp adit execuç prest cont selec inform registr aba formal cas duvid pers gentil entr contat</t>
-  </si>
-  <si>
-    <t>venh através dest solic public sistem si analis api ja disponi homolog fs lan appweb hom hom iissqlnumer siaianaliseapihom</t>
+    <t>prez bom dia acontec mens tant aba adit execuc prest cont dev proced grat vez ajud respost ant inser dad camp adit execuc prest cont selec inform registr aba formal cas duvid pers gentil entr contat</t>
+  </si>
+  <si>
+    <t>venh atraves dest solic public sistem si analis api ja disponi homolog fs lan appweb hom hom iissqlnumer siaianaliseapihom</t>
   </si>
   <si>
     <t>configur token</t>
   </si>
   <si>
-    <t>clic registr nao estp traz institu ensin pré cadastr clic dand err sess invál</t>
-  </si>
-  <si>
-    <t>possível conclu cadastr port design ser usu gerenci encaminh conform port n numer numer tc</t>
+    <t>clic registr nao estp traz institu ensin pre cadastr clic dand err sess inval</t>
+  </si>
+  <si>
+    <t>possivel conclu cadastr port design ser usu gerenci encaminh conform port n numer numer tc</t>
   </si>
   <si>
     <t>substitu nobreak</t>
@@ -835,19 +835,19 @@
     <t>instal comput numer moni numer</t>
   </si>
   <si>
-    <t>venh através dest solic public sistem port etc ja disponi homolog client fs lan appweb hom hom iissqlnumer portaletcehom bast copi past app sobrescrev past environment api fs lan appweb hom hom iissqlnumer portaletceapihom copi conteud sobrescrev past config arqu web config</t>
-  </si>
-  <si>
-    <t>instal comput numer moni numer máquin estagi</t>
-  </si>
-  <si>
-    <t>solicit pont red adic comput local coordenad oper crédit extern copcex numer and</t>
+    <t>venh atraves dest solic public sistem port etc ja disponi homolog client fs lan appweb hom hom iissqlnumer portaletcehom bast copi past app sobrescrev past environment api fs lan appweb hom hom iissqlnumer portaletceapihom copi conteud sobrescrev past config arqu web config</t>
+  </si>
+  <si>
+    <t>instal comput numer moni numer maquin estagi</t>
+  </si>
+  <si>
+    <t>solicit pont red adic comput local coordenad oper credit extern copcex numer and</t>
   </si>
   <si>
     <t>instal nobreak mcm numer</t>
   </si>
   <si>
-    <t>aprov solicit funcional códig numer nom mirn ayak silv maruok</t>
+    <t>aprov solicit funcional codig numer nom mirn ayak silv maruok</t>
   </si>
   <si>
     <t>solicit aplic tarj mut dap numer process list planilh anex</t>
@@ -856,22 +856,22 @@
     <t>instal nobreak mcm numer estagi</t>
   </si>
   <si>
-    <t>senh dire solicit voss senh provid quant cadastr estagiár francilen dia canindé perfil acess padr estagi acess ambi virtual dad diret dad fge coorden cont gest bem acess past red dest diret solicit aind provid cadastr fim biometr registr frequ pont</t>
+    <t>senh dire solicit voss senh provid quant cadastr estagiar francilen dia caninde perfil acess padr estagi acess ambi virtual dad diret dad fge coorden cont gest bem acess past red dest diret solicit aind provid cadastr fim biometr registr frequ pont</t>
   </si>
   <si>
     <t>solicit instal sistem ergon</t>
   </si>
   <si>
-    <t>alt eraç oper cpf numer nom daniel cosm rodrig</t>
+    <t>alt erac oper cpf numer nom daniel cosm rodrig</t>
   </si>
   <si>
     <t>solicit confer mater receb almoxarif refer nf numer macrosolution</t>
   </si>
   <si>
-    <t>senh dire cient determin impost cort cont espec cont control relacion seguranç comun v sa exclus serv daniel cosm rodrig cpf numer tod sistem tce rn part dia numer numer numer términ ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informá provid cab</t>
-  </si>
-  <si>
-    <t>senh dire vis autu facilit anális process cont govern numer di sug din proced desenvolv ferrament process autu seguint sequ event numer cap event numer ppa event numer ldo event numer loa event numer crédit adic event numer di pca</t>
+    <t>senh dire cient determin impost cort cont espec cont control relacion seguranc comun v sa exclus serv daniel cosm rodrig cpf numer tod sistem tce rn part dia numer numer numer termin ativ atual camp bloquei sim exclus set set atual indef realiz ativ nest cort cont desd ent cient respons comun diret informa provid cab</t>
+  </si>
+  <si>
+    <t>senh dire vis autu facilit analis process cont govern numer di sug din proced desenvolv ferrament process autu seguint sequ event numer cap event numer ppa event numer ldo event numer loa event numer credit adic event numer di pca</t>
   </si>
   <si>
     <t>instal pje configur soc</t>
@@ -883,16 +883,16 @@
     <t>cadastr oper cpf numer nom mar gabriell so gom</t>
   </si>
   <si>
-    <t>dire expedi relat atend solicit inform diret conseg efetu cadastr document process ano diverg corr dev tr seguranç exist sistem process dest form solicit diret informá desenvolv ferrament possibilit tip cadastr natal numer setembr numer michely gom araúj dire expedi cient dess inform ord conselh rela pres process solicit provid afim liber funcional soluç conveni</t>
+    <t>dire expedi relat atend solicit inform diret conseg efetu cadastr document process ano diverg corr dev tr seguranc exist sistem process dest form solicit diret informa desenvolv ferrament possibilit tip cadastr natal numer setembr numer michely gom arauj dire expedi cient dess inform ord conselh rela pres process solicit provid afim liber funcional soluc conveni</t>
   </si>
   <si>
     <t>configur comput</t>
   </si>
   <si>
-    <t>aprov solicit funcional códig numer nom mar gabriell so gom</t>
-  </si>
-  <si>
-    <t>ord organiz cabe energ red recepç geral tribun</t>
+    <t>aprov solicit funcional codig numer nom mar gabriell so gom</t>
+  </si>
+  <si>
+    <t>ord organiz cabe energ red recepc geral tribun</t>
   </si>
   <si>
     <t>seg imag err backup anex tent abr anex numer err apresent</t>
@@ -904,13 +904,13 @@
     <t>usu solicit auxili imprim fatur</t>
   </si>
   <si>
-    <t>aprov solicit funcional códig numer nom ilcen mar franç lim</t>
-  </si>
-  <si>
-    <t>cumpr estil solicit instal si colet máquin utiliz dire dam</t>
-  </si>
-  <si>
-    <t>ord coorden geral solicit v sa autoriz set compet dest diret realiz cadastr áre restrit biometr estagiár mar gabriell so gom cpf n numer numer numer regular junt set estági dest tribun lot nest escol cont part hoj</t>
+    <t>aprov solicit funcional codig numer nom ilcen mar franc lim</t>
+  </si>
+  <si>
+    <t>cumpr estil solicit instal si colet maquin utiliz dire dam</t>
+  </si>
+  <si>
+    <t>ord coorden geral solicit v sa autoriz set compet dest diret realiz cadastr are restrit biometr estagiar mar gabriell so gom cpf n numer numer numer regular junt set estagi dest tribun lot nest escol cont part hoj</t>
   </si>
   <si>
     <t>usu solicit auxili configur scann</t>
@@ -925,10 +925,10 @@
     <t>conseg entr ere restrit</t>
   </si>
   <si>
-    <t>realiz alt eraç pra ue dire poss alt er process ano anteri atual permit efetu dat registr alt eraç dev s ecoloc justif melh</t>
-  </si>
-  <si>
-    <t>melh valid pesso realiz valid pesso via dat registr registr valid document comprobatóri valid deix ger cit notific intim pesso nao sid valid</t>
+    <t>realiz alt erac pra ue dire poss alt er process ano anteri atual permit efetu dat registr alt erac dev s ecoloc justif melh</t>
+  </si>
+  <si>
+    <t>melh valid pesso realiz valid pesso via dat registr registr valid document comprobatori valid deix ger cit notific intim pesso nao sid valid</t>
   </si>
   <si>
     <t>configur ergon</t>
@@ -952,10 +952,10 @@
     <t>tecl pc funcion</t>
   </si>
   <si>
-    <t>exist crit ger anex numer ond ped pra cadastr font mens referenc feit id tabel dest form usu nao conseg realiz correç sab cont precis ser cadastr</t>
-  </si>
-  <si>
-    <t>felip per anex qua numer set numer numer numer hor si bom dia envi si relat numer bimestr numer prefeit josé seridó ocorr sistem apresent err atíp diz val pag bimestr inferi val inform bimestr anteri pod ser vist abaix contud inform corret desp pag dur mê mai numer estorn dia numer numer numer empenh numer estorn ocorr ness dot porqu serv apresent document justific utiliz diár receb val empenh liquid pag estorn nenhum empenh dot numer julh agost ness projet numer real val acumul fic inferi bimestr anteri log solicit corrig process equivoc inform anex enc comprov anális atencios felip per med crít s arqu lrf prefeit municip josé seridó numer numer anex numer balanç orçament receit desp err numer val pag bimestr atual rcifra numer numer men val pag inform envi bimestr anteri rcifra numer numer códig desp numer numer numer códig projet ativ numer</t>
+    <t>exist crit ger anex numer ond ped pra cadastr font mens referenc feit id tabel dest form usu nao conseg realiz correc sab cont precis ser cadastr</t>
+  </si>
+  <si>
+    <t>felip per anex qua numer set numer numer numer hor si bom dia envi si relat numer bimestr numer prefeit jose serido ocorr sistem apresent err atip diz val pag bimestr inferi val inform bimestr anteri pod ser vist abaix contud inform corret desp pag dur me mai numer estorn dia numer numer numer empenh numer estorn ocorr ness dot porqu serv apresent document justific utiliz diar receb val empenh liquid pag estorn nenhum empenh dot numer julh agost ness projet numer real val acumul fic inferi bimestr anteri log solicit corrig process equivoc inform anex enc comprov analis atencios felip per med crit s arqu lrf prefeit municip jose serido numer numer anex numer balanc orcament receit desp err numer val pag bimestr atual rcifra numer numer men val pag inform envi bimestr anteri rcifra numer numer codig desp numer numer numer codig projet ativ numer</t>
   </si>
   <si>
     <t>apoi operac</t>
@@ -967,10 +967,10 @@
     <t>memor numer numer exist doi anex anex declaracp apresent err tent visual serv err in arearestrit application configuration err description an err occurred during the processing of configuration fil required to serv thil request pleas review the specific err detail below and modify your configuration fil appropriately pars err messag an err occurred loading configuration fil failed to start monitoring chang to numer numer tcecifra informaco arearestrit becaus acces is denied sourc err an application err occurred on the serv the current custom err setting thil application prevent the detail of the application err from being viewed remotely security reasom it could howev be viewed by brows running on the local serv machin sourc fil numer numer tcecifra informaco arearestrit web config lin numer version information microsoft net framework version numer numer asp net version numer numer</t>
   </si>
   <si>
-    <t>inclu seguint opç fundament legal ferrament complement ato civil artig numer incis iii alíne b constitu estad civil artig numer incis iii alíne d constitu estad</t>
-  </si>
-  <si>
-    <t>consult envi comprov public rre rgf ano numer prefeit arê vê seguint mens seg anex solicit regular intuít visual anex</t>
+    <t>inclu seguint opc fundament legal ferrament complement ato civil artig numer incis iii aline b constitu estad civil artig numer incis iii aline d constitu estad</t>
+  </si>
+  <si>
+    <t>consult envi comprov public rre rgf ano numer prefeit are ve seguint mens seg anex solicit regular intuit visual anex</t>
   </si>
   <si>
     <t>problem assin inform</t>
@@ -997,7 +997,7 @@
     <t>valid not fiscal eb numer estabiliz</t>
   </si>
   <si>
-    <t>valid not fiscal marcrosolution peç scann</t>
+    <t>valid not fiscal marcrosolution pec scann</t>
   </si>
   <si>
     <t>usu esta duvid crit process port ges inform usu err val somat ori inform q nao et corret</t>
@@ -1009,10 +1009,10 @@
     <t>necess instal extens inser inform process</t>
   </si>
   <si>
-    <t>usuár duvid val coloc camp val anex numer val mens total inform val ser inform dev ser total</t>
-  </si>
-  <si>
-    <t>alt eraç oper cpf numer nom francisc azeved</t>
+    <t>usuar duvid val coloc camp val anex numer val mens total inform val ser inform dev ser total</t>
+  </si>
+  <si>
+    <t>alt erac oper cpf numer nom francisc azeved</t>
   </si>
 </sst>
 </file>

</xml_diff>